<commit_message>
Added logger and ThreadLocalDriver
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/testdata/loginTestData.xlsx
+++ b/src/main/java/com/qa/testdata/loginTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lakshmy-SeleniumWorkSpace\OpenCartTest\src\main\java\com\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7853C821-209E-45B8-88DE-55B38825E3A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754489B3-B710-4B6A-B63F-B0B93818162A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{9F16C835-A618-441D-913D-7482C88E8F34}"/>
+    <workbookView xWindow="2160" yWindow="2160" windowWidth="14400" windowHeight="7290" xr2:uid="{9F16C835-A618-441D-913D-7482C88E8F34}"/>
   </bookViews>
   <sheets>
     <sheet name="loginData" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -525,7 +525,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>